<commit_message>
adicinando botao de saida
</commit_message>
<xml_diff>
--- a/data/base_dizimos.xlsx
+++ b/data/base_dizimos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,250 +468,26 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>pastor joaa</t>
+          <t>valdirene</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2345,00</t>
+          <t>150,00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>23,00</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>ef</t>
-        </is>
-      </c>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>22/02/2026 17:19:29</t>
+          <t>23/02/2026 01:15:46</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
-        <is>
-          <t>ADMINISTRADOR</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>23,00</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>23,00</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>22/02/2026 17:25:29</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>ADMINISTRADOR</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>jorje</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>34,00</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>34,00</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>22/02/2026 17:27:11</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>ADMINISTRADOR</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>denis</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>244,00</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>353,00</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>22/02/2026 17:28:22</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>daniel novais</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>dede</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>33,00</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>33,00</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>22/02/2026 17:29:13</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>daniel novais</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>32,00</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>323,00</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>22/02/2026 17:36:17</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>ADMINISTRADOR</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>oooo</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>333,00</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>333,00</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>333</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>22/02/2026 18:22:14</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>daniel novais</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>rr</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>33,00</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0,00</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>22/02/2026 18:48:02</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
         <is>
           <t>ADMINISTRADOR</t>
         </is>

</xml_diff>